<commit_message>
Function Description sheet 추가
</commit_message>
<xml_diff>
--- a/0_DOC/Plasma_Gen_Functioin List_20180104.xlsx
+++ b/0_DOC/Plasma_Gen_Functioin List_20180104.xlsx
@@ -4,17 +4,18 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Function List" sheetId="1" r:id="rId1"/>
+    <sheet name="Function Description" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="135">
   <si>
     <t>No</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -373,6 +374,205 @@
   </si>
   <si>
     <t>-</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Off 상태에서 KEY를 3sec 이상 누른 경우 Power On</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>On 상태에서 KEY를 3sec 이상 누른 경우 Power Off</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>OK</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Normal 상태 - BLUE LED</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">완충 상태 - Green LED </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>충전 상태 - RED LED</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Low battery - Red Blink</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>전원 On/Off 상태 표시
+충전 및 충전지 상태 표시</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>On going</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>+8V On / Off control</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PWM Pulse 1,2 (80KHz) On/Off control</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Plasma ON LED</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Plasma On시 LED ON</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Plasma On time을 5단계로 조정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Level-1 : 2msec On / 8msec Off</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Level-2 : 4msec On / 6msec Off</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Level-3 : 6msec On / 4msec Off</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Level-4 : 8msec On / 2msec Off</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Level-5 : 항상 On ( 10msec On / 0msec Off )</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Power On : Sound 1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Power Off : Sound 2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Plasma On/Off : Sound 3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>H/W reset</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Battery</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4.2V 1A 이상 사용</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Battery CON 지원</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>thermistor Pin 지원</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Battery 온도 monitor를 위한 ADC monitor</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Battery voltage 상태 check를 위한 ADC monitor</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>충전/완충 상태 monitor</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Battery 4.2V까지 충전을 위한 IC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>충전중 Battery 온도 Over시 충전 차단</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DC/DC Converter</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3.3V의 고정 전압 사용</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Plasma 전원 - Transformer 전압용</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>USB CON을 통해 충전</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>플라즈마 생성을 위한 승압용 Boost Converter - 8V , 1A 이상</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>9-pin D-Sub CON</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Board Control를 위한 Interface</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Option : USB D+/D-도 사용가능하도록 설계</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>F/W download용 커넥터</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4-Pin CON 지원 ( w/o RESET-Pin )</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Operation</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Comment</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Buzzer</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>기능 구현 필요</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>H/W optimize 필요</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ADC check 필요</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>알람 사운드용 Buzzer
+ - Power On/Off 상태 알람
+ - Plasma On/Off 상태 알람</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -380,7 +580,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -420,6 +620,15 @@
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -435,7 +644,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="19">
+  <borders count="36">
     <border>
       <left/>
       <right/>
@@ -693,11 +902,238 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -798,26 +1234,155 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1128,8 +1693,8 @@
   </sheetPr>
   <dimension ref="B1:J22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1152,35 +1717,35 @@
         <v>16</v>
       </c>
       <c r="D2" s="2"/>
-      <c r="I2" s="34" t="s">
+      <c r="I2" s="66" t="s">
         <v>80</v>
       </c>
-      <c r="J2" s="35"/>
+      <c r="J2" s="67"/>
     </row>
     <row r="3" spans="2:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="36" t="s">
+      <c r="B3" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="38" t="s">
+      <c r="C3" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="38" t="s">
+      <c r="D3" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="38" t="s">
+      <c r="E3" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="39" t="s">
+      <c r="F3" s="65" t="s">
         <v>23</v>
       </c>
-      <c r="G3" s="39"/>
-      <c r="H3" s="40" t="s">
+      <c r="G3" s="65"/>
+      <c r="H3" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="I3" s="36" t="s">
+      <c r="I3" s="34" t="s">
         <v>81</v>
       </c>
-      <c r="J3" s="37" t="s">
+      <c r="J3" s="35" t="s">
         <v>82</v>
       </c>
     </row>
@@ -1744,4 +2309,635 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="84" fitToHeight="0" orientation="landscape" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="B1:H33"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J17" sqref="J17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="2.625" customWidth="1"/>
+    <col min="2" max="2" width="9" style="1"/>
+    <col min="3" max="3" width="17.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32.75" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="57.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.5" customWidth="1"/>
+    <col min="7" max="7" width="14.625" customWidth="1"/>
+    <col min="8" max="8" width="24.125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:8" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:8" ht="21" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="66" t="s">
+        <v>80</v>
+      </c>
+      <c r="G2" s="67"/>
+    </row>
+    <row r="3" spans="2:8" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="34" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="37" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="37" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="39" t="s">
+        <v>128</v>
+      </c>
+      <c r="F3" s="34" t="s">
+        <v>81</v>
+      </c>
+      <c r="G3" s="35" t="s">
+        <v>82</v>
+      </c>
+      <c r="H3" s="56" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B4" s="81">
+        <v>1</v>
+      </c>
+      <c r="C4" s="82" t="s">
+        <v>43</v>
+      </c>
+      <c r="D4" s="82" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="52" t="s">
+        <v>86</v>
+      </c>
+      <c r="F4" s="53" t="s">
+        <v>88</v>
+      </c>
+      <c r="G4" s="54" t="s">
+        <v>88</v>
+      </c>
+      <c r="H4" s="57"/>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B5" s="70"/>
+      <c r="C5" s="73"/>
+      <c r="D5" s="73"/>
+      <c r="E5" s="40" t="s">
+        <v>87</v>
+      </c>
+      <c r="F5" s="23" t="s">
+        <v>83</v>
+      </c>
+      <c r="G5" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="H5" s="58"/>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B6" s="79">
+        <v>2</v>
+      </c>
+      <c r="C6" s="77" t="s">
+        <v>44</v>
+      </c>
+      <c r="D6" s="83" t="s">
+        <v>93</v>
+      </c>
+      <c r="E6" s="46" t="s">
+        <v>89</v>
+      </c>
+      <c r="F6" s="23" t="s">
+        <v>83</v>
+      </c>
+      <c r="G6" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="H6" s="59"/>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B7" s="79"/>
+      <c r="C7" s="77"/>
+      <c r="D7" s="77"/>
+      <c r="E7" s="46" t="s">
+        <v>90</v>
+      </c>
+      <c r="F7" s="23" t="s">
+        <v>83</v>
+      </c>
+      <c r="G7" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="H7" s="59"/>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B8" s="79"/>
+      <c r="C8" s="77"/>
+      <c r="D8" s="77"/>
+      <c r="E8" s="46" t="s">
+        <v>91</v>
+      </c>
+      <c r="F8" s="23" t="s">
+        <v>83</v>
+      </c>
+      <c r="G8" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="H8" s="59"/>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B9" s="79"/>
+      <c r="C9" s="77"/>
+      <c r="D9" s="77"/>
+      <c r="E9" s="46" t="s">
+        <v>92</v>
+      </c>
+      <c r="F9" s="23" t="s">
+        <v>83</v>
+      </c>
+      <c r="G9" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="H9" s="60"/>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B10" s="3">
+        <v>3</v>
+      </c>
+      <c r="C10" s="50" t="s">
+        <v>59</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="E10" s="46" t="s">
+        <v>108</v>
+      </c>
+      <c r="F10" s="23" t="s">
+        <v>83</v>
+      </c>
+      <c r="G10" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="H10" s="59"/>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B11" s="79">
+        <v>4</v>
+      </c>
+      <c r="C11" s="77" t="s">
+        <v>45</v>
+      </c>
+      <c r="D11" s="78" t="s">
+        <v>34</v>
+      </c>
+      <c r="E11" s="47" t="s">
+        <v>95</v>
+      </c>
+      <c r="F11" s="23" t="s">
+        <v>83</v>
+      </c>
+      <c r="G11" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="H11" s="61"/>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B12" s="79"/>
+      <c r="C12" s="77"/>
+      <c r="D12" s="78"/>
+      <c r="E12" s="48" t="s">
+        <v>96</v>
+      </c>
+      <c r="F12" s="23" t="s">
+        <v>83</v>
+      </c>
+      <c r="G12" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="H12" s="62"/>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B13" s="3">
+        <v>5</v>
+      </c>
+      <c r="C13" s="50" t="s">
+        <v>97</v>
+      </c>
+      <c r="D13" s="45" t="s">
+        <v>35</v>
+      </c>
+      <c r="E13" s="48" t="s">
+        <v>98</v>
+      </c>
+      <c r="F13" s="23" t="s">
+        <v>83</v>
+      </c>
+      <c r="G13" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="H13" s="62"/>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B14" s="79">
+        <v>6</v>
+      </c>
+      <c r="C14" s="77" t="s">
+        <v>46</v>
+      </c>
+      <c r="D14" s="80" t="s">
+        <v>99</v>
+      </c>
+      <c r="E14" s="49" t="s">
+        <v>100</v>
+      </c>
+      <c r="F14" s="23" t="s">
+        <v>83</v>
+      </c>
+      <c r="G14" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="H14" s="63"/>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B15" s="79"/>
+      <c r="C15" s="77"/>
+      <c r="D15" s="80"/>
+      <c r="E15" s="49" t="s">
+        <v>101</v>
+      </c>
+      <c r="F15" s="23" t="s">
+        <v>83</v>
+      </c>
+      <c r="G15" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="H15" s="63"/>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B16" s="79"/>
+      <c r="C16" s="77"/>
+      <c r="D16" s="80"/>
+      <c r="E16" s="49" t="s">
+        <v>102</v>
+      </c>
+      <c r="F16" s="23" t="s">
+        <v>83</v>
+      </c>
+      <c r="G16" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="H16" s="63"/>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B17" s="79"/>
+      <c r="C17" s="77"/>
+      <c r="D17" s="80"/>
+      <c r="E17" s="49" t="s">
+        <v>103</v>
+      </c>
+      <c r="F17" s="23" t="s">
+        <v>83</v>
+      </c>
+      <c r="G17" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="H17" s="63"/>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B18" s="79"/>
+      <c r="C18" s="77"/>
+      <c r="D18" s="80"/>
+      <c r="E18" s="49" t="s">
+        <v>104</v>
+      </c>
+      <c r="F18" s="23" t="s">
+        <v>83</v>
+      </c>
+      <c r="G18" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="H18" s="63"/>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B19" s="68">
+        <v>7</v>
+      </c>
+      <c r="C19" s="71" t="s">
+        <v>130</v>
+      </c>
+      <c r="D19" s="74" t="s">
+        <v>134</v>
+      </c>
+      <c r="E19" s="41" t="s">
+        <v>105</v>
+      </c>
+      <c r="F19" s="23" t="s">
+        <v>83</v>
+      </c>
+      <c r="G19" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="H19" s="60"/>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B20" s="69"/>
+      <c r="C20" s="72"/>
+      <c r="D20" s="76"/>
+      <c r="E20" s="41" t="s">
+        <v>106</v>
+      </c>
+      <c r="F20" s="23" t="s">
+        <v>83</v>
+      </c>
+      <c r="G20" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="H20" s="60"/>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B21" s="69"/>
+      <c r="C21" s="72"/>
+      <c r="D21" s="76"/>
+      <c r="E21" s="41" t="s">
+        <v>107</v>
+      </c>
+      <c r="F21" s="23" t="s">
+        <v>83</v>
+      </c>
+      <c r="G21" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="H21" s="60"/>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B22" s="68">
+        <v>8</v>
+      </c>
+      <c r="C22" s="71" t="s">
+        <v>109</v>
+      </c>
+      <c r="D22" s="74" t="s">
+        <v>110</v>
+      </c>
+      <c r="E22" s="41" t="s">
+        <v>111</v>
+      </c>
+      <c r="F22" s="23" t="s">
+        <v>83</v>
+      </c>
+      <c r="G22" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="H22" s="60"/>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B23" s="69"/>
+      <c r="C23" s="72"/>
+      <c r="D23" s="75"/>
+      <c r="E23" s="41" t="s">
+        <v>114</v>
+      </c>
+      <c r="F23" s="43" t="s">
+        <v>94</v>
+      </c>
+      <c r="G23" s="44" t="s">
+        <v>94</v>
+      </c>
+      <c r="H23" s="60" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B24" s="70"/>
+      <c r="C24" s="73"/>
+      <c r="D24" s="51" t="s">
+        <v>112</v>
+      </c>
+      <c r="E24" s="41" t="s">
+        <v>113</v>
+      </c>
+      <c r="F24" s="43" t="s">
+        <v>94</v>
+      </c>
+      <c r="G24" s="44" t="s">
+        <v>94</v>
+      </c>
+      <c r="H24" s="60" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B25" s="68">
+        <v>9</v>
+      </c>
+      <c r="C25" s="71" t="s">
+        <v>49</v>
+      </c>
+      <c r="D25" s="74" t="s">
+        <v>116</v>
+      </c>
+      <c r="E25" s="41" t="s">
+        <v>121</v>
+      </c>
+      <c r="F25" s="23" t="s">
+        <v>83</v>
+      </c>
+      <c r="G25" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="H25" s="60"/>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B26" s="69"/>
+      <c r="C26" s="72"/>
+      <c r="D26" s="76"/>
+      <c r="E26" s="41" t="s">
+        <v>115</v>
+      </c>
+      <c r="F26" s="23" t="s">
+        <v>83</v>
+      </c>
+      <c r="G26" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="H26" s="60"/>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B27" s="70"/>
+      <c r="C27" s="73"/>
+      <c r="D27" s="75"/>
+      <c r="E27" s="41" t="s">
+        <v>117</v>
+      </c>
+      <c r="F27" s="43" t="s">
+        <v>94</v>
+      </c>
+      <c r="G27" s="44" t="s">
+        <v>94</v>
+      </c>
+      <c r="H27" s="60" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B28" s="68">
+        <v>10</v>
+      </c>
+      <c r="C28" s="71" t="s">
+        <v>118</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="E28" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="F28" s="23" t="s">
+        <v>83</v>
+      </c>
+      <c r="G28" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="H28" s="60"/>
+    </row>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B29" s="69"/>
+      <c r="C29" s="72"/>
+      <c r="D29" s="71" t="s">
+        <v>120</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="F29" s="23" t="s">
+        <v>83</v>
+      </c>
+      <c r="G29" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="H29" s="59"/>
+    </row>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B30" s="70"/>
+      <c r="C30" s="73"/>
+      <c r="D30" s="73"/>
+      <c r="E30" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="F30" s="43" t="s">
+        <v>94</v>
+      </c>
+      <c r="G30" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="H30" s="60" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="31" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B31" s="68">
+        <v>11</v>
+      </c>
+      <c r="C31" s="71" t="s">
+        <v>51</v>
+      </c>
+      <c r="D31" s="74" t="s">
+        <v>124</v>
+      </c>
+      <c r="E31" s="41" t="s">
+        <v>123</v>
+      </c>
+      <c r="F31" s="43" t="s">
+        <v>94</v>
+      </c>
+      <c r="G31" s="44" t="s">
+        <v>94</v>
+      </c>
+      <c r="H31" s="60" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="32" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B32" s="70"/>
+      <c r="C32" s="73"/>
+      <c r="D32" s="75"/>
+      <c r="E32" s="41" t="s">
+        <v>125</v>
+      </c>
+      <c r="F32" s="43" t="s">
+        <v>94</v>
+      </c>
+      <c r="G32" s="44" t="s">
+        <v>94</v>
+      </c>
+      <c r="H32" s="60" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="33" spans="2:8" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B33" s="13">
+        <v>12</v>
+      </c>
+      <c r="C33" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="D33" s="55" t="s">
+        <v>126</v>
+      </c>
+      <c r="E33" s="42" t="s">
+        <v>127</v>
+      </c>
+      <c r="F33" s="25" t="s">
+        <v>83</v>
+      </c>
+      <c r="G33" s="26" t="s">
+        <v>83</v>
+      </c>
+      <c r="H33" s="64"/>
+    </row>
+  </sheetData>
+  <mergeCells count="28">
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="D6:D9"/>
+    <mergeCell ref="C6:C9"/>
+    <mergeCell ref="B6:B9"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="B14:B18"/>
+    <mergeCell ref="C14:C18"/>
+    <mergeCell ref="D14:D18"/>
+    <mergeCell ref="B25:B27"/>
+    <mergeCell ref="C25:C27"/>
+    <mergeCell ref="D25:D27"/>
+    <mergeCell ref="D19:D21"/>
+    <mergeCell ref="C19:C21"/>
+    <mergeCell ref="B19:B21"/>
+    <mergeCell ref="B22:B24"/>
+    <mergeCell ref="D22:D23"/>
+    <mergeCell ref="C22:C24"/>
+    <mergeCell ref="B28:B30"/>
+    <mergeCell ref="C28:C30"/>
+    <mergeCell ref="D29:D30"/>
+    <mergeCell ref="D31:D32"/>
+    <mergeCell ref="C31:C32"/>
+    <mergeCell ref="B31:B32"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="84" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
DOC - Plasma Off sound 삭제
</commit_message>
<xml_diff>
--- a/0_DOC/Plasma_Gen_Functioin List_20180104.xlsx
+++ b/0_DOC/Plasma_Gen_Functioin List_20180104.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12060" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Function List" sheetId="1" r:id="rId1"/>
@@ -462,10 +462,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Plasma On/Off : Sound 3</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>H/W reset</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -572,7 +568,11 @@
   <si>
     <t>알람 사운드용 Buzzer
  - Power On/Off 상태 알람
- - Plasma On/Off 상태 알람</t>
+ - Plasma On 상태 알람</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Plasma On : Sound 3</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1336,13 +1336,37 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1351,37 +1375,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2319,7 +2319,7 @@
   <dimension ref="B1:H33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2355,7 +2355,7 @@
         <v>3</v>
       </c>
       <c r="E3" s="39" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F3" s="34" t="s">
         <v>81</v>
@@ -2364,17 +2364,17 @@
         <v>82</v>
       </c>
       <c r="H3" s="56" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B4" s="81">
+      <c r="B4" s="68">
         <v>1</v>
       </c>
-      <c r="C4" s="82" t="s">
+      <c r="C4" s="70" t="s">
         <v>43</v>
       </c>
-      <c r="D4" s="82" t="s">
+      <c r="D4" s="70" t="s">
         <v>6</v>
       </c>
       <c r="E4" s="52" t="s">
@@ -2389,9 +2389,9 @@
       <c r="H4" s="57"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B5" s="70"/>
-      <c r="C5" s="73"/>
-      <c r="D5" s="73"/>
+      <c r="B5" s="69"/>
+      <c r="C5" s="71"/>
+      <c r="D5" s="71"/>
       <c r="E5" s="40" t="s">
         <v>87</v>
       </c>
@@ -2404,13 +2404,13 @@
       <c r="H5" s="58"/>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B6" s="79">
+      <c r="B6" s="74">
         <v>2</v>
       </c>
-      <c r="C6" s="77" t="s">
+      <c r="C6" s="73" t="s">
         <v>44</v>
       </c>
-      <c r="D6" s="83" t="s">
+      <c r="D6" s="72" t="s">
         <v>93</v>
       </c>
       <c r="E6" s="46" t="s">
@@ -2425,9 +2425,9 @@
       <c r="H6" s="59"/>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B7" s="79"/>
-      <c r="C7" s="77"/>
-      <c r="D7" s="77"/>
+      <c r="B7" s="74"/>
+      <c r="C7" s="73"/>
+      <c r="D7" s="73"/>
       <c r="E7" s="46" t="s">
         <v>90</v>
       </c>
@@ -2440,9 +2440,9 @@
       <c r="H7" s="59"/>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B8" s="79"/>
-      <c r="C8" s="77"/>
-      <c r="D8" s="77"/>
+      <c r="B8" s="74"/>
+      <c r="C8" s="73"/>
+      <c r="D8" s="73"/>
       <c r="E8" s="46" t="s">
         <v>91</v>
       </c>
@@ -2455,9 +2455,9 @@
       <c r="H8" s="59"/>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B9" s="79"/>
-      <c r="C9" s="77"/>
-      <c r="D9" s="77"/>
+      <c r="B9" s="74"/>
+      <c r="C9" s="73"/>
+      <c r="D9" s="73"/>
       <c r="E9" s="46" t="s">
         <v>92</v>
       </c>
@@ -2480,7 +2480,7 @@
         <v>39</v>
       </c>
       <c r="E10" s="46" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F10" s="23" t="s">
         <v>83</v>
@@ -2491,13 +2491,13 @@
       <c r="H10" s="59"/>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B11" s="79">
+      <c r="B11" s="74">
         <v>4</v>
       </c>
-      <c r="C11" s="77" t="s">
+      <c r="C11" s="73" t="s">
         <v>45</v>
       </c>
-      <c r="D11" s="78" t="s">
+      <c r="D11" s="75" t="s">
         <v>34</v>
       </c>
       <c r="E11" s="47" t="s">
@@ -2512,9 +2512,9 @@
       <c r="H11" s="61"/>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B12" s="79"/>
-      <c r="C12" s="77"/>
-      <c r="D12" s="78"/>
+      <c r="B12" s="74"/>
+      <c r="C12" s="73"/>
+      <c r="D12" s="75"/>
       <c r="E12" s="48" t="s">
         <v>96</v>
       </c>
@@ -2548,13 +2548,13 @@
       <c r="H13" s="62"/>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B14" s="79">
+      <c r="B14" s="74">
         <v>6</v>
       </c>
-      <c r="C14" s="77" t="s">
+      <c r="C14" s="73" t="s">
         <v>46</v>
       </c>
-      <c r="D14" s="80" t="s">
+      <c r="D14" s="76" t="s">
         <v>99</v>
       </c>
       <c r="E14" s="49" t="s">
@@ -2569,9 +2569,9 @@
       <c r="H14" s="63"/>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B15" s="79"/>
-      <c r="C15" s="77"/>
-      <c r="D15" s="80"/>
+      <c r="B15" s="74"/>
+      <c r="C15" s="73"/>
+      <c r="D15" s="76"/>
       <c r="E15" s="49" t="s">
         <v>101</v>
       </c>
@@ -2584,9 +2584,9 @@
       <c r="H15" s="63"/>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B16" s="79"/>
-      <c r="C16" s="77"/>
-      <c r="D16" s="80"/>
+      <c r="B16" s="74"/>
+      <c r="C16" s="73"/>
+      <c r="D16" s="76"/>
       <c r="E16" s="49" t="s">
         <v>102</v>
       </c>
@@ -2599,9 +2599,9 @@
       <c r="H16" s="63"/>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B17" s="79"/>
-      <c r="C17" s="77"/>
-      <c r="D17" s="80"/>
+      <c r="B17" s="74"/>
+      <c r="C17" s="73"/>
+      <c r="D17" s="76"/>
       <c r="E17" s="49" t="s">
         <v>103</v>
       </c>
@@ -2614,9 +2614,9 @@
       <c r="H17" s="63"/>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B18" s="79"/>
-      <c r="C18" s="77"/>
-      <c r="D18" s="80"/>
+      <c r="B18" s="74"/>
+      <c r="C18" s="73"/>
+      <c r="D18" s="76"/>
       <c r="E18" s="49" t="s">
         <v>104</v>
       </c>
@@ -2629,14 +2629,14 @@
       <c r="H18" s="63"/>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B19" s="68">
+      <c r="B19" s="77">
         <v>7</v>
       </c>
-      <c r="C19" s="71" t="s">
-        <v>130</v>
-      </c>
-      <c r="D19" s="74" t="s">
-        <v>134</v>
+      <c r="C19" s="79" t="s">
+        <v>129</v>
+      </c>
+      <c r="D19" s="81" t="s">
+        <v>133</v>
       </c>
       <c r="E19" s="41" t="s">
         <v>105</v>
@@ -2650,9 +2650,9 @@
       <c r="H19" s="60"/>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B20" s="69"/>
-      <c r="C20" s="72"/>
-      <c r="D20" s="76"/>
+      <c r="B20" s="78"/>
+      <c r="C20" s="80"/>
+      <c r="D20" s="82"/>
       <c r="E20" s="41" t="s">
         <v>106</v>
       </c>
@@ -2665,11 +2665,11 @@
       <c r="H20" s="60"/>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B21" s="69"/>
-      <c r="C21" s="72"/>
-      <c r="D21" s="76"/>
+      <c r="B21" s="78"/>
+      <c r="C21" s="80"/>
+      <c r="D21" s="82"/>
       <c r="E21" s="41" t="s">
-        <v>107</v>
+        <v>134</v>
       </c>
       <c r="F21" s="23" t="s">
         <v>83</v>
@@ -2680,18 +2680,18 @@
       <c r="H21" s="60"/>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B22" s="68">
+      <c r="B22" s="77">
         <v>8</v>
       </c>
-      <c r="C22" s="71" t="s">
+      <c r="C22" s="79" t="s">
+        <v>108</v>
+      </c>
+      <c r="D22" s="81" t="s">
         <v>109</v>
       </c>
-      <c r="D22" s="74" t="s">
+      <c r="E22" s="41" t="s">
         <v>110</v>
       </c>
-      <c r="E22" s="41" t="s">
-        <v>111</v>
-      </c>
       <c r="F22" s="23" t="s">
         <v>83</v>
       </c>
@@ -2701,11 +2701,11 @@
       <c r="H22" s="60"/>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B23" s="69"/>
-      <c r="C23" s="72"/>
-      <c r="D23" s="75"/>
+      <c r="B23" s="78"/>
+      <c r="C23" s="80"/>
+      <c r="D23" s="83"/>
       <c r="E23" s="41" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F23" s="43" t="s">
         <v>94</v>
@@ -2714,17 +2714,17 @@
         <v>94</v>
       </c>
       <c r="H23" s="60" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B24" s="70"/>
-      <c r="C24" s="73"/>
+      <c r="B24" s="69"/>
+      <c r="C24" s="71"/>
       <c r="D24" s="51" t="s">
+        <v>111</v>
+      </c>
+      <c r="E24" s="41" t="s">
         <v>112</v>
-      </c>
-      <c r="E24" s="41" t="s">
-        <v>113</v>
       </c>
       <c r="F24" s="43" t="s">
         <v>94</v>
@@ -2733,51 +2733,51 @@
         <v>94</v>
       </c>
       <c r="H24" s="60" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B25" s="68">
+      <c r="B25" s="77">
         <v>9</v>
       </c>
-      <c r="C25" s="71" t="s">
+      <c r="C25" s="79" t="s">
         <v>49</v>
       </c>
-      <c r="D25" s="74" t="s">
+      <c r="D25" s="81" t="s">
+        <v>115</v>
+      </c>
+      <c r="E25" s="41" t="s">
+        <v>120</v>
+      </c>
+      <c r="F25" s="23" t="s">
+        <v>83</v>
+      </c>
+      <c r="G25" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="H25" s="60"/>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B26" s="78"/>
+      <c r="C26" s="80"/>
+      <c r="D26" s="82"/>
+      <c r="E26" s="41" t="s">
+        <v>114</v>
+      </c>
+      <c r="F26" s="23" t="s">
+        <v>83</v>
+      </c>
+      <c r="G26" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="H26" s="60"/>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B27" s="69"/>
+      <c r="C27" s="71"/>
+      <c r="D27" s="83"/>
+      <c r="E27" s="41" t="s">
         <v>116</v>
-      </c>
-      <c r="E25" s="41" t="s">
-        <v>121</v>
-      </c>
-      <c r="F25" s="23" t="s">
-        <v>83</v>
-      </c>
-      <c r="G25" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="H25" s="60"/>
-    </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B26" s="69"/>
-      <c r="C26" s="72"/>
-      <c r="D26" s="76"/>
-      <c r="E26" s="41" t="s">
-        <v>115</v>
-      </c>
-      <c r="F26" s="23" t="s">
-        <v>83</v>
-      </c>
-      <c r="G26" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="H26" s="60"/>
-    </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B27" s="70"/>
-      <c r="C27" s="73"/>
-      <c r="D27" s="75"/>
-      <c r="E27" s="41" t="s">
-        <v>117</v>
       </c>
       <c r="F27" s="43" t="s">
         <v>94</v>
@@ -2786,35 +2786,35 @@
         <v>94</v>
       </c>
       <c r="H27" s="60" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B28" s="68">
+      <c r="B28" s="77">
         <v>10</v>
       </c>
-      <c r="C28" s="71" t="s">
-        <v>118</v>
+      <c r="C28" s="79" t="s">
+        <v>117</v>
       </c>
       <c r="D28" s="4" t="s">
         <v>48</v>
       </c>
       <c r="E28" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="F28" s="23" t="s">
+        <v>83</v>
+      </c>
+      <c r="G28" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="H28" s="60"/>
+    </row>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B29" s="78"/>
+      <c r="C29" s="80"/>
+      <c r="D29" s="79" t="s">
         <v>119</v>
-      </c>
-      <c r="F28" s="23" t="s">
-        <v>83</v>
-      </c>
-      <c r="G28" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="H28" s="60"/>
-    </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B29" s="69"/>
-      <c r="C29" s="72"/>
-      <c r="D29" s="71" t="s">
-        <v>120</v>
       </c>
       <c r="E29" s="4" t="s">
         <v>54</v>
@@ -2828,11 +2828,11 @@
       <c r="H29" s="59"/>
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B30" s="70"/>
-      <c r="C30" s="73"/>
-      <c r="D30" s="73"/>
+      <c r="B30" s="69"/>
+      <c r="C30" s="71"/>
+      <c r="D30" s="71"/>
       <c r="E30" s="6" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F30" s="43" t="s">
         <v>94</v>
@@ -2841,21 +2841,21 @@
         <v>83</v>
       </c>
       <c r="H30" s="60" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="31" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B31" s="68">
+      <c r="B31" s="77">
         <v>11</v>
       </c>
-      <c r="C31" s="71" t="s">
+      <c r="C31" s="79" t="s">
         <v>51</v>
       </c>
-      <c r="D31" s="74" t="s">
-        <v>124</v>
+      <c r="D31" s="81" t="s">
+        <v>123</v>
       </c>
       <c r="E31" s="41" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F31" s="43" t="s">
         <v>94</v>
@@ -2864,15 +2864,15 @@
         <v>94</v>
       </c>
       <c r="H31" s="60" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="32" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B32" s="70"/>
-      <c r="C32" s="73"/>
-      <c r="D32" s="75"/>
+      <c r="B32" s="69"/>
+      <c r="C32" s="71"/>
+      <c r="D32" s="83"/>
       <c r="E32" s="41" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F32" s="43" t="s">
         <v>94</v>
@@ -2881,7 +2881,7 @@
         <v>94</v>
       </c>
       <c r="H32" s="60" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="33" spans="2:8" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
@@ -2892,10 +2892,10 @@
         <v>57</v>
       </c>
       <c r="D33" s="55" t="s">
+        <v>125</v>
+      </c>
+      <c r="E33" s="42" t="s">
         <v>126</v>
-      </c>
-      <c r="E33" s="42" t="s">
-        <v>127</v>
       </c>
       <c r="F33" s="25" t="s">
         <v>83</v>
@@ -2907,19 +2907,12 @@
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="D6:D9"/>
-    <mergeCell ref="C6:C9"/>
-    <mergeCell ref="B6:B9"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="B14:B18"/>
-    <mergeCell ref="C14:C18"/>
-    <mergeCell ref="D14:D18"/>
+    <mergeCell ref="B28:B30"/>
+    <mergeCell ref="C28:C30"/>
+    <mergeCell ref="D29:D30"/>
+    <mergeCell ref="D31:D32"/>
+    <mergeCell ref="C31:C32"/>
+    <mergeCell ref="B31:B32"/>
     <mergeCell ref="B25:B27"/>
     <mergeCell ref="C25:C27"/>
     <mergeCell ref="D25:D27"/>
@@ -2929,12 +2922,19 @@
     <mergeCell ref="B22:B24"/>
     <mergeCell ref="D22:D23"/>
     <mergeCell ref="C22:C24"/>
-    <mergeCell ref="B28:B30"/>
-    <mergeCell ref="C28:C30"/>
-    <mergeCell ref="D29:D30"/>
-    <mergeCell ref="D31:D32"/>
-    <mergeCell ref="C31:C32"/>
-    <mergeCell ref="B31:B32"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="B14:B18"/>
+    <mergeCell ref="C14:C18"/>
+    <mergeCell ref="D14:D18"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="D6:D9"/>
+    <mergeCell ref="C6:C9"/>
+    <mergeCell ref="B6:B9"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
DOC - Function list update
</commit_message>
<xml_diff>
--- a/0_DOC/Plasma_Gen_Functioin List_20180104.xlsx
+++ b/0_DOC/Plasma_Gen_Functioin List_20180104.xlsx
@@ -9,13 +9,17 @@
   <sheets>
     <sheet name="Function List" sheetId="1" r:id="rId1"/>
     <sheet name="Function Description" sheetId="2" r:id="rId2"/>
+    <sheet name="Flow chart" sheetId="3" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="2">'Flow chart'!$A$1:$N$30</definedName>
+  </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="134">
   <si>
     <t>No</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -346,13 +350,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>알람 사운드용 부져
- - Power On
- - Power Off
- - Low battery</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>기능검사</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -366,14 +363,6 @@
   </si>
   <si>
     <t>OK</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>On going</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>-</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -482,14 +471,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Battery 온도 monitor를 위한 ADC monitor</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Battery voltage 상태 check를 위한 ADC monitor</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>충전/완충 상태 monitor</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -498,10 +479,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>충전중 Battery 온도 Over시 충전 차단</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>DC/DC Converter</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -559,10 +536,6 @@
   </si>
   <si>
     <t>H/W optimize 필요</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ADC check 필요</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -573,6 +546,35 @@
   </si>
   <si>
     <t>Plasma On : Sound 3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>알람 사운드용 부져
+ - Power On/Off
+ - Plasma On</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Plasma Generator flow chart</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Battery voltage 상태 check를 위한 ADC monitor
+ - 완충 : 4.2V
+ - Low battery : 3.4V</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>충전중 Battery 온도 Over시 충전 차단
+ - operating temperature range : -10℃ ~ 60℃</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Battery 온도 monitor를 위한 ADC monitor</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ADC optimize 필요</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -644,7 +646,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="36">
+  <borders count="32">
     <border>
       <left/>
       <right/>
@@ -743,32 +745,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color auto="1"/>
       </left>
@@ -824,9 +800,26 @@
       <left style="thin">
         <color auto="1"/>
       </left>
-      <right/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
       <top/>
       <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
         <color auto="1"/>
       </bottom>
       <diagonal/>
@@ -835,50 +828,9 @@
       <left style="thin">
         <color auto="1"/>
       </left>
-      <right style="medium">
+      <right style="thin">
         <color auto="1"/>
       </right>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
       <top style="medium">
         <color auto="1"/>
       </top>
@@ -1133,7 +1085,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="84">
+  <cellXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1189,200 +1141,189 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1399,6 +1340,1470 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>493055</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>29884</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>440574</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>48934</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="모서리가 둥근 직사각형 3"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="493055" y="2797737"/>
+          <a:ext cx="1998195" cy="870697"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent6">
+            <a:lumMod val="40000"/>
+            <a:lumOff val="60000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="ko-KR" altLang="en-US" sz="1100" b="1" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>전원 </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ko-KR" sz="1100" b="1" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>OFF </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ko-KR" altLang="en-US" sz="1100" b="1" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>상태</a:t>
+          </a:r>
+          <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100" b="1">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>509119</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>23909</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>232894</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>25590</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="원호 4"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4610472" y="1514291"/>
+          <a:ext cx="2458010" cy="1917887"/>
+        </a:xfrm>
+        <a:prstGeom prst="arc">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 16200000"/>
+            <a:gd name="adj2" fmla="val 27501"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln w="28575">
+          <a:headEnd type="none" w="med" len="med"/>
+          <a:tailEnd type="triangle" w="med" len="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>293406</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>59021</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>178919</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>98801</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="24" name="그룹 23"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="3027641" y="697756"/>
+          <a:ext cx="2619749" cy="1530163"/>
+          <a:chOff x="3027641" y="451224"/>
+          <a:chExt cx="2619749" cy="1530163"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="2" name="모서리가 둥근 직사각형 1"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="3027641" y="451224"/>
+            <a:ext cx="2619749" cy="1530163"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="accent6">
+              <a:lumMod val="40000"/>
+              <a:lumOff val="60000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr lang="ko-KR" altLang="en-US" sz="1100" b="1" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>전원 </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" altLang="ko-KR" sz="1100" b="1" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>ON</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="ko-KR" altLang="en-US" sz="1100" b="1" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t> 상태</a:t>
+            </a:r>
+            <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:endParaRPr>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="6" name="모서리가 둥근 직사각형 5"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="3256241" y="886573"/>
+            <a:ext cx="2219699" cy="973978"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="accent3">
+              <a:lumMod val="40000"/>
+              <a:lumOff val="60000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:r>
+              <a:rPr lang="en-US" altLang="ko-KR" sz="1100">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Main</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" altLang="ko-KR" sz="1100" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t> </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="ko-KR" altLang="en-US" sz="1100" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>전원 </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" altLang="ko-KR" sz="1100" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>ON</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:r>
+              <a:rPr lang="en-US" altLang="ko-KR" sz="1100" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Buzzer 1 ON</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" altLang="ko-KR" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:endParaRPr>
+          </a:p>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:r>
+              <a:rPr lang="en-US" altLang="ko-KR" sz="1100">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Status</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" altLang="ko-KR" sz="1100" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t> LED : BLUE ON</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:r>
+              <a:rPr lang="en-US" altLang="ko-KR" sz="1100" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>RS-232 ON</a:t>
+            </a:r>
+            <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:endParaRPr>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>423394</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>98801</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>313576</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>117851</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="23" name="그룹 22"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="6575423" y="2653742"/>
+          <a:ext cx="2624418" cy="1509433"/>
+          <a:chOff x="6575423" y="2407210"/>
+          <a:chExt cx="2624418" cy="1509433"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="3" name="모서리가 둥근 직사각형 2"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="6575423" y="2407210"/>
+            <a:ext cx="2624418" cy="1509433"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="accent6">
+              <a:lumMod val="40000"/>
+              <a:lumOff val="60000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr lang="en-US" altLang="ko-KR" sz="1100" b="1">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Plasma</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" altLang="ko-KR" sz="1100" b="1" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t> On </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="ko-KR" altLang="en-US" sz="1100" b="1" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>상태</a:t>
+            </a:r>
+            <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:endParaRPr>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="7" name="모서리가 둥근 직사각형 6"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="6833532" y="2794933"/>
+            <a:ext cx="2226609" cy="1029447"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="accent3">
+              <a:lumMod val="40000"/>
+              <a:lumOff val="60000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:r>
+              <a:rPr lang="en-US" altLang="ko-KR" sz="1100">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>+8V</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" altLang="ko-KR" sz="1100" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t> </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="ko-KR" altLang="en-US" sz="1100" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>전원 </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" altLang="ko-KR" sz="1100" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>ON</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:r>
+              <a:rPr lang="en-US" altLang="ko-KR" sz="1100" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Buzzer 3 ON</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" altLang="ko-KR" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:endParaRPr>
+          </a:p>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:r>
+              <a:rPr lang="en-US" altLang="ko-KR" sz="1100" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Plasam On LED : White ON</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:r>
+              <a:rPr lang="en-US" altLang="ko-KR" sz="1100" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>PWM Pulse 1,2 ON</a:t>
+            </a:r>
+            <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:endParaRPr>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>341031</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>190876</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>223369</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>51176</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="22" name="그룹 21"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="3075266" y="4449111"/>
+          <a:ext cx="2616574" cy="1563594"/>
+          <a:chOff x="3075266" y="4202579"/>
+          <a:chExt cx="2616574" cy="1563594"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="8" name="모서리가 둥근 직사각형 7"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="3075266" y="4202579"/>
+            <a:ext cx="2616574" cy="1563594"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="accent6">
+              <a:lumMod val="40000"/>
+              <a:lumOff val="60000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr lang="ko-KR" altLang="en-US" sz="1100" b="1">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>충전 상태</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="9" name="모서리가 둥근 직사각형 8"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="3295275" y="4596840"/>
+            <a:ext cx="2218765" cy="1070909"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="accent3">
+              <a:lumMod val="40000"/>
+              <a:lumOff val="60000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:r>
+              <a:rPr lang="en-US" altLang="ko-KR" sz="1100">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Status</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" altLang="ko-KR" sz="1100" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t> LED : </a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:r>
+              <a:rPr lang="en-US" altLang="ko-KR" sz="1100" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>   - </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="ko-KR" altLang="en-US" sz="1100" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>충전중 </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" altLang="ko-KR" sz="1100" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>: RED ON</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:r>
+              <a:rPr lang="en-US" altLang="ko-KR" sz="1100" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>   - </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="ko-KR" altLang="en-US" sz="1100" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>완충 </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" altLang="ko-KR" sz="1100" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>: GREEN ON</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:r>
+              <a:rPr lang="en-US" altLang="ko-KR" sz="1100" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Battery Temp monitor</a:t>
+            </a:r>
+            <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:endParaRPr>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>204319</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>173507</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>536013</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>25589</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10" name="원호 9"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4305672" y="1238066"/>
+          <a:ext cx="3065929" cy="2407023"/>
+        </a:xfrm>
+        <a:prstGeom prst="arc">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 16200000"/>
+            <a:gd name="adj2" fmla="val 27501"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln w="28575">
+          <a:headEnd type="triangle" w="med" len="med"/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>614828</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>198720</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1140312" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="11" name="TextBox 10"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6766857" y="1263279"/>
+          <a:ext cx="1140312" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ko-KR" sz="1100"/>
+            <a:t>Plasma</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ko-KR" sz="1100" baseline="0"/>
+            <a:t> Key Push</a:t>
+          </a:r>
+          <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>347194</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>198720</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1140312" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="12" name="TextBox 11"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5815665" y="1902014"/>
+          <a:ext cx="1140312" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ko-KR" sz="1100"/>
+            <a:t>Plasma</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ko-KR" sz="1100" baseline="0"/>
+            <a:t> Key Push</a:t>
+          </a:r>
+          <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>299569</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>189196</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>26519</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>190876</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="13" name="원호 12"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="1666687" y="1679578"/>
+          <a:ext cx="2461185" cy="1917886"/>
+        </a:xfrm>
+        <a:prstGeom prst="arc">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 16200000"/>
+            <a:gd name="adj2" fmla="val 27501"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln w="28575">
+          <a:headEnd type="none" w="med" len="med"/>
+          <a:tailEnd type="triangle" w="med" len="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>676460</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>129057</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>328144</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>190876</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="14" name="원호 13"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="1360019" y="1406528"/>
+          <a:ext cx="3069478" cy="2403848"/>
+        </a:xfrm>
+        <a:prstGeom prst="arc">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 16200000"/>
+            <a:gd name="adj2" fmla="val 27501"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln w="28575">
+          <a:headEnd type="triangle" w="med" len="med"/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>332626</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>189195</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1457579" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="15" name="TextBox 14"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1016185" y="1253754"/>
+          <a:ext cx="1457579" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ko-KR" sz="1100" baseline="0"/>
+            <a:t>Power Key Push : 3sec</a:t>
+          </a:r>
+          <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>423394</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>60701</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1457579" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="16" name="TextBox 15"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1790512" y="2189819"/>
+          <a:ext cx="1457579" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ko-KR" sz="1100" baseline="0"/>
+            <a:t>Power Key Push : 3sec</a:t>
+          </a:r>
+          <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>189751</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>190876</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1104470" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="17" name="TextBox 16"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="2923986" y="3171641"/>
+          <a:ext cx="1104470" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ko-KR" sz="1100"/>
+            <a:t>USB Connection</a:t>
+          </a:r>
+          <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>537694</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>209926</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1263231" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="18" name="TextBox 17"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="4639047" y="3190691"/>
+          <a:ext cx="1263231" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ko-KR" sz="1100"/>
+            <a:t>USB Disconnection</a:t>
+          </a:r>
+          <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>332066</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>3177</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1104470" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="19" name="TextBox 18"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="1015625" y="1067736"/>
+          <a:ext cx="1104470" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ko-KR" sz="1100"/>
+            <a:t>USB Connection</a:t>
+          </a:r>
+          <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>619871</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>38851</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>619871</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>22789</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="20" name="직선 화살표 연결선 19"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4037665" y="2380880"/>
+          <a:ext cx="0" cy="1900144"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575">
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>514162</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>38851</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>514162</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>22789</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="21" name="직선 화살표 연결선 20"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4615515" y="2380880"/>
+          <a:ext cx="0" cy="1900144"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575">
+          <a:headEnd type="triangle" w="med" len="med"/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1691,10 +3096,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:J22"/>
+  <dimension ref="B2:H22"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="E31" sqref="E31:E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1707,79 +3112,60 @@
     <col min="6" max="6" width="17.125" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8.875" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="20.625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.5" customWidth="1"/>
-    <col min="10" max="10" width="14.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:10" ht="21" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:8" ht="21" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B2" s="7" t="s">
         <v>16</v>
       </c>
       <c r="D2" s="2"/>
-      <c r="I2" s="66" t="s">
-        <v>80</v>
-      </c>
-      <c r="J2" s="67"/>
-    </row>
-    <row r="3" spans="2:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="34" t="s">
+    </row>
+    <row r="3" spans="2:8" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="36" t="s">
+      <c r="C3" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="36" t="s">
+      <c r="D3" s="55" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="36" t="s">
+      <c r="E3" s="55" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="65" t="s">
+      <c r="F3" s="58" t="s">
         <v>23</v>
       </c>
-      <c r="G3" s="65"/>
-      <c r="H3" s="38" t="s">
+      <c r="G3" s="58"/>
+      <c r="H3" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="I3" s="34" t="s">
-        <v>81</v>
-      </c>
-      <c r="J3" s="35" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B4" s="27">
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B4" s="56">
         <v>1</v>
       </c>
-      <c r="C4" s="28" t="s">
+      <c r="C4" s="22" t="s">
         <v>42</v>
       </c>
-      <c r="D4" s="29">
+      <c r="D4" s="23">
         <v>1</v>
       </c>
-      <c r="E4" s="28" t="s">
+      <c r="E4" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="30" t="s">
+      <c r="F4" s="24" t="s">
         <v>67</v>
       </c>
-      <c r="G4" s="30" t="s">
+      <c r="G4" s="24" t="s">
         <v>68</v>
       </c>
-      <c r="H4" s="31" t="s">
+      <c r="H4" s="77" t="s">
         <v>66</v>
       </c>
-      <c r="I4" s="32" t="s">
-        <v>84</v>
-      </c>
-      <c r="J4" s="33" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B5" s="3">
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B5" s="57">
         <v>2</v>
       </c>
       <c r="C5" s="4" t="s">
@@ -1797,18 +3183,12 @@
       <c r="G5" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="H5" s="19" t="s">
+      <c r="H5" s="78" t="s">
         <v>64</v>
       </c>
-      <c r="I5" s="23" t="s">
-        <v>83</v>
-      </c>
-      <c r="J5" s="12" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="6" spans="2:10" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="B6" s="3">
+    </row>
+    <row r="6" spans="2:8" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="B6" s="57">
         <v>3</v>
       </c>
       <c r="C6" s="4" t="s">
@@ -1826,18 +3206,12 @@
       <c r="G6" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="H6" s="20" t="s">
+      <c r="H6" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="I6" s="23" t="s">
-        <v>83</v>
-      </c>
-      <c r="J6" s="12" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B7" s="3">
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B7" s="57">
         <v>4</v>
       </c>
       <c r="C7" s="4" t="s">
@@ -1855,18 +3229,12 @@
       <c r="G7" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="H7" s="19" t="s">
+      <c r="H7" s="78" t="s">
         <v>64</v>
       </c>
-      <c r="I7" s="23" t="s">
-        <v>83</v>
-      </c>
-      <c r="J7" s="12" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B8" s="3">
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B8" s="57">
         <v>5</v>
       </c>
       <c r="C8" s="4" t="s">
@@ -1884,18 +3252,12 @@
       <c r="G8" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="H8" s="19" t="s">
+      <c r="H8" s="78" t="s">
         <v>69</v>
       </c>
-      <c r="I8" s="23" t="s">
-        <v>83</v>
-      </c>
-      <c r="J8" s="12" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B9" s="3">
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B9" s="57">
         <v>6</v>
       </c>
       <c r="C9" s="4" t="s">
@@ -1913,18 +3275,12 @@
       <c r="G9" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="H9" s="19" t="s">
+      <c r="H9" s="78" t="s">
         <v>70</v>
       </c>
-      <c r="I9" s="23" t="s">
-        <v>83</v>
-      </c>
-      <c r="J9" s="12" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="10" spans="2:10" ht="66" x14ac:dyDescent="0.3">
-      <c r="B10" s="3">
+    </row>
+    <row r="10" spans="2:8" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="B10" s="57">
         <v>7</v>
       </c>
       <c r="C10" s="4" t="s">
@@ -1934,7 +3290,7 @@
         <v>1</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>79</v>
+        <v>128</v>
       </c>
       <c r="F10" s="5" t="s">
         <v>18</v>
@@ -1942,18 +3298,12 @@
       <c r="G10" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="H10" s="19" t="s">
+      <c r="H10" s="78" t="s">
         <v>8</v>
       </c>
-      <c r="I10" s="23" t="s">
-        <v>83</v>
-      </c>
-      <c r="J10" s="12" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="11" spans="2:10" ht="33" x14ac:dyDescent="0.3">
-      <c r="B11" s="3">
+    </row>
+    <row r="11" spans="2:8" ht="33" x14ac:dyDescent="0.3">
+      <c r="B11" s="57">
         <v>8</v>
       </c>
       <c r="C11" s="4" t="s">
@@ -1971,18 +3321,12 @@
       <c r="G11" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="H11" s="19" t="s">
+      <c r="H11" s="78" t="s">
         <v>10</v>
       </c>
-      <c r="I11" s="23" t="s">
-        <v>83</v>
-      </c>
-      <c r="J11" s="12" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="12" spans="2:10" ht="33" x14ac:dyDescent="0.3">
-      <c r="B12" s="3">
+    </row>
+    <row r="12" spans="2:8" ht="33" x14ac:dyDescent="0.3">
+      <c r="B12" s="57">
         <v>9</v>
       </c>
       <c r="C12" s="4" t="s">
@@ -2000,18 +3344,12 @@
       <c r="G12" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="H12" s="19" t="s">
+      <c r="H12" s="78" t="s">
         <v>11</v>
       </c>
-      <c r="I12" s="23" t="s">
-        <v>83</v>
-      </c>
-      <c r="J12" s="12" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B13" s="3">
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B13" s="57">
         <v>10</v>
       </c>
       <c r="C13" s="4" t="s">
@@ -2029,18 +3367,12 @@
       <c r="G13" s="16" t="s">
         <v>73</v>
       </c>
-      <c r="H13" s="19" t="s">
+      <c r="H13" s="78" t="s">
         <v>63</v>
       </c>
-      <c r="I13" s="23" t="s">
-        <v>83</v>
-      </c>
-      <c r="J13" s="12" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="14" spans="2:10" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="B14" s="3">
+    </row>
+    <row r="14" spans="2:8" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="B14" s="57">
         <v>11</v>
       </c>
       <c r="C14" s="4" t="s">
@@ -2058,18 +3390,12 @@
       <c r="G14" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="H14" s="19" t="s">
+      <c r="H14" s="78" t="s">
         <v>62</v>
       </c>
-      <c r="I14" s="23" t="s">
-        <v>84</v>
-      </c>
-      <c r="J14" s="12" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B15" s="3">
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B15" s="57">
         <v>12</v>
       </c>
       <c r="C15" s="4" t="s">
@@ -2087,18 +3413,12 @@
       <c r="G15" s="16" t="s">
         <v>73</v>
       </c>
-      <c r="H15" s="20" t="s">
+      <c r="H15" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="I15" s="23" t="s">
-        <v>83</v>
-      </c>
-      <c r="J15" s="24" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="16" spans="2:10" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="B16" s="3">
+    </row>
+    <row r="16" spans="2:8" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="B16" s="57">
         <v>13</v>
       </c>
       <c r="C16" s="4" t="s">
@@ -2116,18 +3436,12 @@
       <c r="G16" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="H16" s="19" t="s">
+      <c r="H16" s="78" t="s">
         <v>61</v>
       </c>
-      <c r="I16" s="23" t="s">
-        <v>84</v>
-      </c>
-      <c r="J16" s="12" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B17" s="3">
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B17" s="57">
         <v>14</v>
       </c>
       <c r="C17" s="4" t="s">
@@ -2145,18 +3459,12 @@
       <c r="G17" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="H17" s="19" t="s">
+      <c r="H17" s="78" t="s">
         <v>71</v>
       </c>
-      <c r="I17" s="23" t="s">
-        <v>83</v>
-      </c>
-      <c r="J17" s="12" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="18" spans="2:10" ht="33" x14ac:dyDescent="0.3">
-      <c r="B18" s="3">
+    </row>
+    <row r="18" spans="2:8" ht="33" x14ac:dyDescent="0.3">
+      <c r="B18" s="57">
         <v>15</v>
       </c>
       <c r="C18" s="4" t="s">
@@ -2174,18 +3482,12 @@
       <c r="G18" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="H18" s="19" t="s">
+      <c r="H18" s="78" t="s">
         <v>72</v>
       </c>
-      <c r="I18" s="23" t="s">
-        <v>83</v>
-      </c>
-      <c r="J18" s="24" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="19" spans="2:10" ht="33" x14ac:dyDescent="0.3">
-      <c r="B19" s="3">
+    </row>
+    <row r="19" spans="2:8" ht="33" x14ac:dyDescent="0.3">
+      <c r="B19" s="57">
         <v>16</v>
       </c>
       <c r="C19" s="4" t="s">
@@ -2203,18 +3505,12 @@
       <c r="G19" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="H19" s="21" t="s">
+      <c r="H19" s="79" t="s">
         <v>13</v>
       </c>
-      <c r="I19" s="23" t="s">
-        <v>83</v>
-      </c>
-      <c r="J19" s="12" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B20" s="3">
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B20" s="57">
         <v>17</v>
       </c>
       <c r="C20" s="4" t="s">
@@ -2232,18 +3528,12 @@
       <c r="G20" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="H20" s="21" t="s">
+      <c r="H20" s="79" t="s">
         <v>13</v>
       </c>
-      <c r="I20" s="23" t="s">
-        <v>83</v>
-      </c>
-      <c r="J20" s="12" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="21" spans="2:10" ht="33" x14ac:dyDescent="0.3">
-      <c r="B21" s="3">
+    </row>
+    <row r="21" spans="2:8" ht="33" x14ac:dyDescent="0.3">
+      <c r="B21" s="57">
         <v>18</v>
       </c>
       <c r="C21" s="4" t="s">
@@ -2261,17 +3551,11 @@
       <c r="G21" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="H21" s="19" t="s">
+      <c r="H21" s="78" t="s">
         <v>72</v>
       </c>
-      <c r="I21" s="23" t="s">
-        <v>83</v>
-      </c>
-      <c r="J21" s="24" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="22" spans="2:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="22" spans="2:8" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B22" s="13">
         <v>19</v>
       </c>
@@ -2290,20 +3574,13 @@
       <c r="G22" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="H22" s="22" t="s">
+      <c r="H22" s="80" t="s">
         <v>41</v>
       </c>
-      <c r="I22" s="25" t="s">
-        <v>83</v>
-      </c>
-      <c r="J22" s="26" t="s">
-        <v>83</v>
-      </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="1">
     <mergeCell ref="F3:G3"/>
-    <mergeCell ref="I2:J2"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2318,8 +3595,8 @@
   </sheetPr>
   <dimension ref="B1:H33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J32" sqref="J32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2339,549 +3616,547 @@
       <c r="B2" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="66" t="s">
+      <c r="F2" s="59" t="s">
+        <v>79</v>
+      </c>
+      <c r="G2" s="60"/>
+    </row>
+    <row r="3" spans="2:8" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="27" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="28" t="s">
+        <v>121</v>
+      </c>
+      <c r="F3" s="25" t="s">
         <v>80</v>
       </c>
-      <c r="G2" s="67"/>
-    </row>
-    <row r="3" spans="2:8" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="34" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="37" t="s">
+      <c r="G3" s="26" t="s">
+        <v>81</v>
+      </c>
+      <c r="H3" s="45" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B4" s="74">
         <v>1</v>
       </c>
-      <c r="D3" s="37" t="s">
-        <v>3</v>
-      </c>
-      <c r="E3" s="39" t="s">
-        <v>127</v>
-      </c>
-      <c r="F3" s="34" t="s">
-        <v>81</v>
-      </c>
-      <c r="G3" s="35" t="s">
-        <v>82</v>
-      </c>
-      <c r="H3" s="56" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B4" s="68">
-        <v>1</v>
-      </c>
-      <c r="C4" s="70" t="s">
+      <c r="C4" s="75" t="s">
         <v>43</v>
       </c>
-      <c r="D4" s="70" t="s">
+      <c r="D4" s="75" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="52" t="s">
+      <c r="E4" s="41" t="s">
+        <v>83</v>
+      </c>
+      <c r="F4" s="42" t="s">
+        <v>85</v>
+      </c>
+      <c r="G4" s="43" t="s">
+        <v>85</v>
+      </c>
+      <c r="H4" s="46"/>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B5" s="63"/>
+      <c r="C5" s="66"/>
+      <c r="D5" s="66"/>
+      <c r="E5" s="29" t="s">
+        <v>84</v>
+      </c>
+      <c r="F5" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="G5" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="H5" s="47"/>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B6" s="72">
+        <v>2</v>
+      </c>
+      <c r="C6" s="70" t="s">
+        <v>44</v>
+      </c>
+      <c r="D6" s="76" t="s">
+        <v>90</v>
+      </c>
+      <c r="E6" s="35" t="s">
         <v>86</v>
       </c>
-      <c r="F4" s="53" t="s">
+      <c r="F6" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="G6" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="H6" s="48"/>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B7" s="72"/>
+      <c r="C7" s="70"/>
+      <c r="D7" s="70"/>
+      <c r="E7" s="35" t="s">
+        <v>87</v>
+      </c>
+      <c r="F7" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="G7" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="H7" s="48"/>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B8" s="72"/>
+      <c r="C8" s="70"/>
+      <c r="D8" s="70"/>
+      <c r="E8" s="35" t="s">
         <v>88</v>
       </c>
-      <c r="G4" s="54" t="s">
-        <v>88</v>
-      </c>
-      <c r="H4" s="57"/>
-    </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B5" s="69"/>
-      <c r="C5" s="71"/>
-      <c r="D5" s="71"/>
-      <c r="E5" s="40" t="s">
-        <v>87</v>
-      </c>
-      <c r="F5" s="23" t="s">
-        <v>83</v>
-      </c>
-      <c r="G5" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="H5" s="58"/>
-    </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B6" s="74">
-        <v>2</v>
-      </c>
-      <c r="C6" s="73" t="s">
-        <v>44</v>
-      </c>
-      <c r="D6" s="72" t="s">
-        <v>93</v>
-      </c>
-      <c r="E6" s="46" t="s">
+      <c r="F8" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="G8" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="H8" s="48"/>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B9" s="72"/>
+      <c r="C9" s="70"/>
+      <c r="D9" s="70"/>
+      <c r="E9" s="35" t="s">
         <v>89</v>
       </c>
-      <c r="F6" s="23" t="s">
-        <v>83</v>
-      </c>
-      <c r="G6" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="H6" s="59"/>
-    </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B7" s="74"/>
-      <c r="C7" s="73"/>
-      <c r="D7" s="73"/>
-      <c r="E7" s="46" t="s">
-        <v>90</v>
-      </c>
-      <c r="F7" s="23" t="s">
-        <v>83</v>
-      </c>
-      <c r="G7" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="H7" s="59"/>
-    </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B8" s="74"/>
-      <c r="C8" s="73"/>
-      <c r="D8" s="73"/>
-      <c r="E8" s="46" t="s">
-        <v>91</v>
-      </c>
-      <c r="F8" s="23" t="s">
-        <v>83</v>
-      </c>
-      <c r="G8" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="H8" s="59"/>
-    </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B9" s="74"/>
-      <c r="C9" s="73"/>
-      <c r="D9" s="73"/>
-      <c r="E9" s="46" t="s">
-        <v>92</v>
-      </c>
-      <c r="F9" s="23" t="s">
-        <v>83</v>
+      <c r="F9" s="19" t="s">
+        <v>82</v>
       </c>
       <c r="G9" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="H9" s="60"/>
+        <v>82</v>
+      </c>
+      <c r="H9" s="49"/>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B10" s="3">
         <v>3</v>
       </c>
-      <c r="C10" s="50" t="s">
+      <c r="C10" s="39" t="s">
         <v>59</v>
       </c>
       <c r="D10" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="E10" s="46" t="s">
-        <v>107</v>
-      </c>
-      <c r="F10" s="23" t="s">
-        <v>83</v>
+      <c r="E10" s="35" t="s">
+        <v>104</v>
+      </c>
+      <c r="F10" s="19" t="s">
+        <v>82</v>
       </c>
       <c r="G10" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="H10" s="59"/>
+        <v>82</v>
+      </c>
+      <c r="H10" s="48"/>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B11" s="74">
+      <c r="B11" s="72">
         <v>4</v>
       </c>
-      <c r="C11" s="73" t="s">
+      <c r="C11" s="70" t="s">
         <v>45</v>
       </c>
-      <c r="D11" s="75" t="s">
+      <c r="D11" s="71" t="s">
         <v>34</v>
       </c>
-      <c r="E11" s="47" t="s">
-        <v>95</v>
-      </c>
-      <c r="F11" s="23" t="s">
-        <v>83</v>
+      <c r="E11" s="36" t="s">
+        <v>92</v>
+      </c>
+      <c r="F11" s="19" t="s">
+        <v>82</v>
       </c>
       <c r="G11" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="H11" s="61"/>
+        <v>82</v>
+      </c>
+      <c r="H11" s="50"/>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B12" s="74"/>
-      <c r="C12" s="73"/>
-      <c r="D12" s="75"/>
-      <c r="E12" s="48" t="s">
-        <v>96</v>
-      </c>
-      <c r="F12" s="23" t="s">
-        <v>83</v>
+      <c r="B12" s="72"/>
+      <c r="C12" s="70"/>
+      <c r="D12" s="71"/>
+      <c r="E12" s="37" t="s">
+        <v>93</v>
+      </c>
+      <c r="F12" s="19" t="s">
+        <v>82</v>
       </c>
       <c r="G12" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="H12" s="62"/>
+        <v>82</v>
+      </c>
+      <c r="H12" s="51"/>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B13" s="3">
         <v>5</v>
       </c>
-      <c r="C13" s="50" t="s">
+      <c r="C13" s="39" t="s">
+        <v>94</v>
+      </c>
+      <c r="D13" s="34" t="s">
+        <v>35</v>
+      </c>
+      <c r="E13" s="37" t="s">
+        <v>95</v>
+      </c>
+      <c r="F13" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="G13" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="H13" s="51"/>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B14" s="72">
+        <v>6</v>
+      </c>
+      <c r="C14" s="70" t="s">
+        <v>46</v>
+      </c>
+      <c r="D14" s="73" t="s">
+        <v>96</v>
+      </c>
+      <c r="E14" s="38" t="s">
         <v>97</v>
       </c>
-      <c r="D13" s="45" t="s">
-        <v>35</v>
-      </c>
-      <c r="E13" s="48" t="s">
+      <c r="F14" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="G14" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="H14" s="52"/>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B15" s="72"/>
+      <c r="C15" s="70"/>
+      <c r="D15" s="73"/>
+      <c r="E15" s="38" t="s">
         <v>98</v>
       </c>
-      <c r="F13" s="23" t="s">
-        <v>83</v>
-      </c>
-      <c r="G13" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="H13" s="62"/>
-    </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B14" s="74">
-        <v>6</v>
-      </c>
-      <c r="C14" s="73" t="s">
-        <v>46</v>
-      </c>
-      <c r="D14" s="76" t="s">
+      <c r="F15" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="G15" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="H15" s="52"/>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B16" s="72"/>
+      <c r="C16" s="70"/>
+      <c r="D16" s="73"/>
+      <c r="E16" s="38" t="s">
         <v>99</v>
       </c>
-      <c r="E14" s="49" t="s">
+      <c r="F16" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="G16" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="H16" s="52"/>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B17" s="72"/>
+      <c r="C17" s="70"/>
+      <c r="D17" s="73"/>
+      <c r="E17" s="38" t="s">
         <v>100</v>
       </c>
-      <c r="F14" s="23" t="s">
-        <v>83</v>
-      </c>
-      <c r="G14" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="H14" s="63"/>
-    </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B15" s="74"/>
-      <c r="C15" s="73"/>
-      <c r="D15" s="76"/>
-      <c r="E15" s="49" t="s">
+      <c r="F17" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="G17" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="H17" s="52"/>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B18" s="72"/>
+      <c r="C18" s="70"/>
+      <c r="D18" s="73"/>
+      <c r="E18" s="38" t="s">
         <v>101</v>
       </c>
-      <c r="F15" s="23" t="s">
-        <v>83</v>
-      </c>
-      <c r="G15" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="H15" s="63"/>
-    </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B16" s="74"/>
-      <c r="C16" s="73"/>
-      <c r="D16" s="76"/>
-      <c r="E16" s="49" t="s">
+      <c r="F18" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="G18" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="H18" s="52"/>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B19" s="61">
+        <v>7</v>
+      </c>
+      <c r="C19" s="64" t="s">
+        <v>123</v>
+      </c>
+      <c r="D19" s="67" t="s">
+        <v>126</v>
+      </c>
+      <c r="E19" s="30" t="s">
         <v>102</v>
       </c>
-      <c r="F16" s="23" t="s">
-        <v>83</v>
-      </c>
-      <c r="G16" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="H16" s="63"/>
-    </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B17" s="74"/>
-      <c r="C17" s="73"/>
-      <c r="D17" s="76"/>
-      <c r="E17" s="49" t="s">
+      <c r="F19" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="G19" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="H19" s="49"/>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B20" s="62"/>
+      <c r="C20" s="65"/>
+      <c r="D20" s="69"/>
+      <c r="E20" s="30" t="s">
         <v>103</v>
       </c>
-      <c r="F17" s="23" t="s">
-        <v>83</v>
-      </c>
-      <c r="G17" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="H17" s="63"/>
-    </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B18" s="74"/>
-      <c r="C18" s="73"/>
-      <c r="D18" s="76"/>
-      <c r="E18" s="49" t="s">
-        <v>104</v>
-      </c>
-      <c r="F18" s="23" t="s">
-        <v>83</v>
-      </c>
-      <c r="G18" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="H18" s="63"/>
-    </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B19" s="77">
-        <v>7</v>
-      </c>
-      <c r="C19" s="79" t="s">
-        <v>129</v>
-      </c>
-      <c r="D19" s="81" t="s">
+      <c r="F20" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="G20" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="H20" s="49"/>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B21" s="62"/>
+      <c r="C21" s="65"/>
+      <c r="D21" s="69"/>
+      <c r="E21" s="30" t="s">
+        <v>127</v>
+      </c>
+      <c r="F21" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="G21" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="H21" s="49"/>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B22" s="61">
+        <v>8</v>
+      </c>
+      <c r="C22" s="64" t="s">
+        <v>105</v>
+      </c>
+      <c r="D22" s="67" t="s">
+        <v>106</v>
+      </c>
+      <c r="E22" s="30" t="s">
+        <v>107</v>
+      </c>
+      <c r="F22" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="G22" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="H22" s="49"/>
+    </row>
+    <row r="23" spans="2:8" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="B23" s="62"/>
+      <c r="C23" s="65"/>
+      <c r="D23" s="68"/>
+      <c r="E23" s="30" t="s">
+        <v>130</v>
+      </c>
+      <c r="F23" s="32" t="s">
+        <v>91</v>
+      </c>
+      <c r="G23" s="33" t="s">
+        <v>91</v>
+      </c>
+      <c r="H23" s="49" t="s">
         <v>133</v>
       </c>
-      <c r="E19" s="41" t="s">
-        <v>105</v>
-      </c>
-      <c r="F19" s="23" t="s">
-        <v>83</v>
-      </c>
-      <c r="G19" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="H19" s="60"/>
-    </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B20" s="78"/>
-      <c r="C20" s="80"/>
-      <c r="D20" s="82"/>
-      <c r="E20" s="41" t="s">
-        <v>106</v>
-      </c>
-      <c r="F20" s="23" t="s">
-        <v>83</v>
-      </c>
-      <c r="G20" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="H20" s="60"/>
-    </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B21" s="78"/>
-      <c r="C21" s="80"/>
-      <c r="D21" s="82"/>
-      <c r="E21" s="41" t="s">
-        <v>134</v>
-      </c>
-      <c r="F21" s="23" t="s">
-        <v>83</v>
-      </c>
-      <c r="G21" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="H21" s="60"/>
-    </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B22" s="77">
-        <v>8</v>
-      </c>
-      <c r="C22" s="79" t="s">
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B24" s="63"/>
+      <c r="C24" s="66"/>
+      <c r="D24" s="40" t="s">
         <v>108</v>
       </c>
-      <c r="D22" s="81" t="s">
+      <c r="E24" s="30" t="s">
+        <v>132</v>
+      </c>
+      <c r="F24" s="32" t="s">
+        <v>91</v>
+      </c>
+      <c r="G24" s="33" t="s">
+        <v>91</v>
+      </c>
+      <c r="H24" s="49" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B25" s="61">
+        <v>9</v>
+      </c>
+      <c r="C25" s="64" t="s">
+        <v>49</v>
+      </c>
+      <c r="D25" s="67" t="s">
+        <v>110</v>
+      </c>
+      <c r="E25" s="30" t="s">
+        <v>114</v>
+      </c>
+      <c r="F25" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="G25" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="H25" s="49"/>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B26" s="62"/>
+      <c r="C26" s="65"/>
+      <c r="D26" s="69"/>
+      <c r="E26" s="30" t="s">
         <v>109</v>
       </c>
-      <c r="E22" s="41" t="s">
-        <v>110</v>
-      </c>
-      <c r="F22" s="23" t="s">
-        <v>83</v>
-      </c>
-      <c r="G22" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="H22" s="60"/>
-    </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B23" s="78"/>
-      <c r="C23" s="80"/>
-      <c r="D23" s="83"/>
-      <c r="E23" s="41" t="s">
-        <v>113</v>
-      </c>
-      <c r="F23" s="43" t="s">
-        <v>94</v>
-      </c>
-      <c r="G23" s="44" t="s">
-        <v>94</v>
-      </c>
-      <c r="H23" s="60" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B24" s="69"/>
-      <c r="C24" s="71"/>
-      <c r="D24" s="51" t="s">
+      <c r="F26" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="G26" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="H26" s="49"/>
+    </row>
+    <row r="27" spans="2:8" ht="33" x14ac:dyDescent="0.3">
+      <c r="B27" s="63"/>
+      <c r="C27" s="66"/>
+      <c r="D27" s="68"/>
+      <c r="E27" s="30" t="s">
+        <v>131</v>
+      </c>
+      <c r="F27" s="32" t="s">
+        <v>91</v>
+      </c>
+      <c r="G27" s="33" t="s">
+        <v>91</v>
+      </c>
+      <c r="H27" s="49" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B28" s="61">
+        <v>10</v>
+      </c>
+      <c r="C28" s="64" t="s">
         <v>111</v>
-      </c>
-      <c r="E24" s="41" t="s">
-        <v>112</v>
-      </c>
-      <c r="F24" s="43" t="s">
-        <v>94</v>
-      </c>
-      <c r="G24" s="44" t="s">
-        <v>94</v>
-      </c>
-      <c r="H24" s="60" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B25" s="77">
-        <v>9</v>
-      </c>
-      <c r="C25" s="79" t="s">
-        <v>49</v>
-      </c>
-      <c r="D25" s="81" t="s">
-        <v>115</v>
-      </c>
-      <c r="E25" s="41" t="s">
-        <v>120</v>
-      </c>
-      <c r="F25" s="23" t="s">
-        <v>83</v>
-      </c>
-      <c r="G25" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="H25" s="60"/>
-    </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B26" s="78"/>
-      <c r="C26" s="80"/>
-      <c r="D26" s="82"/>
-      <c r="E26" s="41" t="s">
-        <v>114</v>
-      </c>
-      <c r="F26" s="23" t="s">
-        <v>83</v>
-      </c>
-      <c r="G26" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="H26" s="60"/>
-    </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B27" s="69"/>
-      <c r="C27" s="71"/>
-      <c r="D27" s="83"/>
-      <c r="E27" s="41" t="s">
-        <v>116</v>
-      </c>
-      <c r="F27" s="43" t="s">
-        <v>94</v>
-      </c>
-      <c r="G27" s="44" t="s">
-        <v>94</v>
-      </c>
-      <c r="H27" s="60" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B28" s="77">
-        <v>10</v>
-      </c>
-      <c r="C28" s="79" t="s">
-        <v>117</v>
       </c>
       <c r="D28" s="4" t="s">
         <v>48</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>118</v>
-      </c>
-      <c r="F28" s="23" t="s">
-        <v>83</v>
+        <v>112</v>
+      </c>
+      <c r="F28" s="19" t="s">
+        <v>82</v>
       </c>
       <c r="G28" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="H28" s="60"/>
+        <v>82</v>
+      </c>
+      <c r="H28" s="49"/>
     </row>
     <row r="29" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B29" s="78"/>
-      <c r="C29" s="80"/>
-      <c r="D29" s="79" t="s">
-        <v>119</v>
+      <c r="B29" s="62"/>
+      <c r="C29" s="65"/>
+      <c r="D29" s="64" t="s">
+        <v>113</v>
       </c>
       <c r="E29" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="F29" s="23" t="s">
-        <v>83</v>
+      <c r="F29" s="19" t="s">
+        <v>82</v>
       </c>
       <c r="G29" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="H29" s="59"/>
+        <v>82</v>
+      </c>
+      <c r="H29" s="48"/>
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B30" s="69"/>
-      <c r="C30" s="71"/>
-      <c r="D30" s="71"/>
+      <c r="B30" s="63"/>
+      <c r="C30" s="66"/>
+      <c r="D30" s="66"/>
       <c r="E30" s="6" t="s">
-        <v>121</v>
-      </c>
-      <c r="F30" s="43" t="s">
-        <v>94</v>
+        <v>115</v>
+      </c>
+      <c r="F30" s="32" t="s">
+        <v>91</v>
       </c>
       <c r="G30" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="H30" s="60" t="s">
-        <v>131</v>
+        <v>82</v>
+      </c>
+      <c r="H30" s="49" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="31" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B31" s="77">
+      <c r="B31" s="61">
         <v>11</v>
       </c>
-      <c r="C31" s="79" t="s">
+      <c r="C31" s="64" t="s">
         <v>51</v>
       </c>
-      <c r="D31" s="81" t="s">
-        <v>123</v>
-      </c>
-      <c r="E31" s="41" t="s">
-        <v>122</v>
-      </c>
-      <c r="F31" s="43" t="s">
-        <v>94</v>
-      </c>
-      <c r="G31" s="44" t="s">
-        <v>94</v>
-      </c>
-      <c r="H31" s="60" t="s">
-        <v>130</v>
-      </c>
+      <c r="D31" s="67" t="s">
+        <v>117</v>
+      </c>
+      <c r="E31" s="30" t="s">
+        <v>116</v>
+      </c>
+      <c r="F31" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="G31" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="H31" s="49"/>
     </row>
     <row r="32" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B32" s="69"/>
-      <c r="C32" s="71"/>
-      <c r="D32" s="83"/>
-      <c r="E32" s="41" t="s">
+      <c r="B32" s="63"/>
+      <c r="C32" s="66"/>
+      <c r="D32" s="68"/>
+      <c r="E32" s="30" t="s">
+        <v>118</v>
+      </c>
+      <c r="F32" s="32" t="s">
+        <v>91</v>
+      </c>
+      <c r="G32" s="33" t="s">
+        <v>91</v>
+      </c>
+      <c r="H32" s="49" t="s">
         <v>124</v>
-      </c>
-      <c r="F32" s="43" t="s">
-        <v>94</v>
-      </c>
-      <c r="G32" s="44" t="s">
-        <v>94</v>
-      </c>
-      <c r="H32" s="60" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="33" spans="2:8" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
@@ -2891,28 +4166,35 @@
       <c r="C33" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="D33" s="55" t="s">
-        <v>125</v>
-      </c>
-      <c r="E33" s="42" t="s">
-        <v>126</v>
-      </c>
-      <c r="F33" s="25" t="s">
-        <v>83</v>
-      </c>
-      <c r="G33" s="26" t="s">
-        <v>83</v>
-      </c>
-      <c r="H33" s="64"/>
+      <c r="D33" s="44" t="s">
+        <v>119</v>
+      </c>
+      <c r="E33" s="31" t="s">
+        <v>120</v>
+      </c>
+      <c r="F33" s="20" t="s">
+        <v>82</v>
+      </c>
+      <c r="G33" s="21" t="s">
+        <v>82</v>
+      </c>
+      <c r="H33" s="53"/>
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="B28:B30"/>
-    <mergeCell ref="C28:C30"/>
-    <mergeCell ref="D29:D30"/>
-    <mergeCell ref="D31:D32"/>
-    <mergeCell ref="C31:C32"/>
-    <mergeCell ref="B31:B32"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="D6:D9"/>
+    <mergeCell ref="C6:C9"/>
+    <mergeCell ref="B6:B9"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="B14:B18"/>
+    <mergeCell ref="C14:C18"/>
+    <mergeCell ref="D14:D18"/>
     <mergeCell ref="B25:B27"/>
     <mergeCell ref="C25:C27"/>
     <mergeCell ref="D25:D27"/>
@@ -2922,22 +4204,41 @@
     <mergeCell ref="B22:B24"/>
     <mergeCell ref="D22:D23"/>
     <mergeCell ref="C22:C24"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="B14:B18"/>
-    <mergeCell ref="C14:C18"/>
-    <mergeCell ref="D14:D18"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="D6:D9"/>
-    <mergeCell ref="C6:C9"/>
-    <mergeCell ref="B6:B9"/>
+    <mergeCell ref="B28:B30"/>
+    <mergeCell ref="C28:C30"/>
+    <mergeCell ref="D29:D30"/>
+    <mergeCell ref="D31:D32"/>
+    <mergeCell ref="C31:C32"/>
+    <mergeCell ref="B31:B32"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="84" fitToHeight="0" orientation="landscape" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView view="pageBreakPreview" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
+      <selection activeCell="K24" sqref="K24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" s="54" t="s">
+        <v>129</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="95" orientation="landscape" r:id="rId1"/>
+  <colBreaks count="1" manualBreakCount="1">
+    <brk id="14" max="1048575" man="1"/>
+  </colBreaks>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
DOC - 1/12 meeting 내용 update
</commit_message>
<xml_diff>
--- a/0_DOC/Plasma_Gen_Functioin List_20180104.xlsx
+++ b/0_DOC/Plasma_Gen_Functioin List_20180104.xlsx
@@ -1,25 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12060" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12060" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Function List" sheetId="1" r:id="rId1"/>
     <sheet name="Function Description" sheetId="2" r:id="rId2"/>
     <sheet name="Flow chart" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="2">'Flow chart'!$A$1:$N$30</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="149">
   <si>
     <t>No</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -575,6 +576,65 @@
   </si>
   <si>
     <t>ADC optimize 필요</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Plasma Gen</t>
+  </si>
+  <si>
+    <t>V1.0</t>
+  </si>
+  <si>
+    <t>Transformer Output check후 마무리</t>
+  </si>
+  <si>
+    <t>V2.0</t>
+  </si>
+  <si>
+    <t>Battery type 과 External Only type 2개 model로 진행</t>
+  </si>
+  <si>
+    <t>F/W는 하나의 version으로 진행</t>
+  </si>
+  <si>
+    <t>H/W model 구별을 위한 ID pin 추가</t>
+  </si>
+  <si>
+    <t>Gas 주입 인식을 위한 GPIO 신호 추가 - 외부에서 입력됨</t>
+  </si>
+  <si>
+    <t>PCB 설계 및 제작 : 4주 ( 각 1ea )</t>
+  </si>
+  <si>
+    <t>M/E data 입수 후 진행
+ 1) PCB 외곽 모양
+ 2) Volume 및 Key 위치
+ 3) Top / Bottom 부품 높이 정보
+ 4) Battery CON 변경 여부 ( 변경시 CON PN 정보 필요)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Plasma LF</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>V1.0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MCU PCB 제작</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>요청 자료
+ - RS-232 통신 : R/Tx data 정보
+ - ADC : 기능 및 data 처리 방법
+ - G17 : 기능 및 처리 방법</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TMS320F2808 Board 입수
+ - CON type : 2.00mm pitch</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1085,7 +1145,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="81">
+  <cellXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1256,54 +1316,70 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1312,18 +1388,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1334,9 +1398,6 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -2849,7 +2910,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2884,7 +2945,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3133,10 +3194,10 @@
       <c r="E3" s="55" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="58" t="s">
+      <c r="F3" s="64" t="s">
         <v>23</v>
       </c>
-      <c r="G3" s="58"/>
+      <c r="G3" s="64"/>
       <c r="H3" s="26" t="s">
         <v>4</v>
       </c>
@@ -3160,7 +3221,7 @@
       <c r="G4" s="24" t="s">
         <v>68</v>
       </c>
-      <c r="H4" s="77" t="s">
+      <c r="H4" s="58" t="s">
         <v>66</v>
       </c>
     </row>
@@ -3183,7 +3244,7 @@
       <c r="G5" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="H5" s="78" t="s">
+      <c r="H5" s="59" t="s">
         <v>64</v>
       </c>
     </row>
@@ -3229,7 +3290,7 @@
       <c r="G7" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="H7" s="78" t="s">
+      <c r="H7" s="59" t="s">
         <v>64</v>
       </c>
     </row>
@@ -3252,7 +3313,7 @@
       <c r="G8" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="H8" s="78" t="s">
+      <c r="H8" s="59" t="s">
         <v>69</v>
       </c>
     </row>
@@ -3275,7 +3336,7 @@
       <c r="G9" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="H9" s="78" t="s">
+      <c r="H9" s="59" t="s">
         <v>70</v>
       </c>
     </row>
@@ -3298,7 +3359,7 @@
       <c r="G10" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="H10" s="78" t="s">
+      <c r="H10" s="59" t="s">
         <v>8</v>
       </c>
     </row>
@@ -3321,7 +3382,7 @@
       <c r="G11" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="H11" s="78" t="s">
+      <c r="H11" s="59" t="s">
         <v>10</v>
       </c>
     </row>
@@ -3344,7 +3405,7 @@
       <c r="G12" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="H12" s="78" t="s">
+      <c r="H12" s="59" t="s">
         <v>11</v>
       </c>
     </row>
@@ -3367,7 +3428,7 @@
       <c r="G13" s="16" t="s">
         <v>73</v>
       </c>
-      <c r="H13" s="78" t="s">
+      <c r="H13" s="59" t="s">
         <v>63</v>
       </c>
     </row>
@@ -3390,7 +3451,7 @@
       <c r="G14" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="H14" s="78" t="s">
+      <c r="H14" s="59" t="s">
         <v>62</v>
       </c>
     </row>
@@ -3436,7 +3497,7 @@
       <c r="G16" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="H16" s="78" t="s">
+      <c r="H16" s="59" t="s">
         <v>61</v>
       </c>
     </row>
@@ -3459,7 +3520,7 @@
       <c r="G17" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="H17" s="78" t="s">
+      <c r="H17" s="59" t="s">
         <v>71</v>
       </c>
     </row>
@@ -3482,7 +3543,7 @@
       <c r="G18" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="H18" s="78" t="s">
+      <c r="H18" s="59" t="s">
         <v>72</v>
       </c>
     </row>
@@ -3505,7 +3566,7 @@
       <c r="G19" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="H19" s="79" t="s">
+      <c r="H19" s="60" t="s">
         <v>13</v>
       </c>
     </row>
@@ -3528,7 +3589,7 @@
       <c r="G20" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="H20" s="79" t="s">
+      <c r="H20" s="60" t="s">
         <v>13</v>
       </c>
     </row>
@@ -3551,7 +3612,7 @@
       <c r="G21" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="H21" s="78" t="s">
+      <c r="H21" s="59" t="s">
         <v>72</v>
       </c>
     </row>
@@ -3574,7 +3635,7 @@
       <c r="G22" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="H22" s="80" t="s">
+      <c r="H22" s="61" t="s">
         <v>41</v>
       </c>
     </row>
@@ -3595,8 +3656,8 @@
   </sheetPr>
   <dimension ref="B1:H33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J32" sqref="J32"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -3616,10 +3677,10 @@
       <c r="B2" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="59" t="s">
+      <c r="F2" s="78" t="s">
         <v>79</v>
       </c>
-      <c r="G2" s="60"/>
+      <c r="G2" s="79"/>
     </row>
     <row r="3" spans="2:8" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="25" t="s">
@@ -3645,13 +3706,13 @@
       </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B4" s="74">
+      <c r="B4" s="80">
         <v>1</v>
       </c>
-      <c r="C4" s="75" t="s">
+      <c r="C4" s="81" t="s">
         <v>43</v>
       </c>
-      <c r="D4" s="75" t="s">
+      <c r="D4" s="81" t="s">
         <v>6</v>
       </c>
       <c r="E4" s="41" t="s">
@@ -3666,9 +3727,9 @@
       <c r="H4" s="46"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B5" s="63"/>
-      <c r="C5" s="66"/>
-      <c r="D5" s="66"/>
+      <c r="B5" s="67"/>
+      <c r="C5" s="70"/>
+      <c r="D5" s="70"/>
       <c r="E5" s="29" t="s">
         <v>84</v>
       </c>
@@ -3681,13 +3742,13 @@
       <c r="H5" s="47"/>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B6" s="72">
+      <c r="B6" s="76">
         <v>2</v>
       </c>
-      <c r="C6" s="70" t="s">
+      <c r="C6" s="74" t="s">
         <v>44</v>
       </c>
-      <c r="D6" s="76" t="s">
+      <c r="D6" s="82" t="s">
         <v>90</v>
       </c>
       <c r="E6" s="35" t="s">
@@ -3702,9 +3763,9 @@
       <c r="H6" s="48"/>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B7" s="72"/>
-      <c r="C7" s="70"/>
-      <c r="D7" s="70"/>
+      <c r="B7" s="76"/>
+      <c r="C7" s="74"/>
+      <c r="D7" s="74"/>
       <c r="E7" s="35" t="s">
         <v>87</v>
       </c>
@@ -3717,9 +3778,9 @@
       <c r="H7" s="48"/>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B8" s="72"/>
-      <c r="C8" s="70"/>
-      <c r="D8" s="70"/>
+      <c r="B8" s="76"/>
+      <c r="C8" s="74"/>
+      <c r="D8" s="74"/>
       <c r="E8" s="35" t="s">
         <v>88</v>
       </c>
@@ -3732,9 +3793,9 @@
       <c r="H8" s="48"/>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B9" s="72"/>
-      <c r="C9" s="70"/>
-      <c r="D9" s="70"/>
+      <c r="B9" s="76"/>
+      <c r="C9" s="74"/>
+      <c r="D9" s="74"/>
       <c r="E9" s="35" t="s">
         <v>89</v>
       </c>
@@ -3768,13 +3829,13 @@
       <c r="H10" s="48"/>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B11" s="72">
+      <c r="B11" s="76">
         <v>4</v>
       </c>
-      <c r="C11" s="70" t="s">
+      <c r="C11" s="74" t="s">
         <v>45</v>
       </c>
-      <c r="D11" s="71" t="s">
+      <c r="D11" s="75" t="s">
         <v>34</v>
       </c>
       <c r="E11" s="36" t="s">
@@ -3789,9 +3850,9 @@
       <c r="H11" s="50"/>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B12" s="72"/>
-      <c r="C12" s="70"/>
-      <c r="D12" s="71"/>
+      <c r="B12" s="76"/>
+      <c r="C12" s="74"/>
+      <c r="D12" s="75"/>
       <c r="E12" s="37" t="s">
         <v>93</v>
       </c>
@@ -3825,13 +3886,13 @@
       <c r="H13" s="51"/>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B14" s="72">
+      <c r="B14" s="76">
         <v>6</v>
       </c>
-      <c r="C14" s="70" t="s">
+      <c r="C14" s="74" t="s">
         <v>46</v>
       </c>
-      <c r="D14" s="73" t="s">
+      <c r="D14" s="77" t="s">
         <v>96</v>
       </c>
       <c r="E14" s="38" t="s">
@@ -3846,9 +3907,9 @@
       <c r="H14" s="52"/>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B15" s="72"/>
-      <c r="C15" s="70"/>
-      <c r="D15" s="73"/>
+      <c r="B15" s="76"/>
+      <c r="C15" s="74"/>
+      <c r="D15" s="77"/>
       <c r="E15" s="38" t="s">
         <v>98</v>
       </c>
@@ -3861,9 +3922,9 @@
       <c r="H15" s="52"/>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B16" s="72"/>
-      <c r="C16" s="70"/>
-      <c r="D16" s="73"/>
+      <c r="B16" s="76"/>
+      <c r="C16" s="74"/>
+      <c r="D16" s="77"/>
       <c r="E16" s="38" t="s">
         <v>99</v>
       </c>
@@ -3876,9 +3937,9 @@
       <c r="H16" s="52"/>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B17" s="72"/>
-      <c r="C17" s="70"/>
-      <c r="D17" s="73"/>
+      <c r="B17" s="76"/>
+      <c r="C17" s="74"/>
+      <c r="D17" s="77"/>
       <c r="E17" s="38" t="s">
         <v>100</v>
       </c>
@@ -3891,9 +3952,9 @@
       <c r="H17" s="52"/>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B18" s="72"/>
-      <c r="C18" s="70"/>
-      <c r="D18" s="73"/>
+      <c r="B18" s="76"/>
+      <c r="C18" s="74"/>
+      <c r="D18" s="77"/>
       <c r="E18" s="38" t="s">
         <v>101</v>
       </c>
@@ -3906,13 +3967,13 @@
       <c r="H18" s="52"/>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B19" s="61">
+      <c r="B19" s="65">
         <v>7</v>
       </c>
-      <c r="C19" s="64" t="s">
+      <c r="C19" s="68" t="s">
         <v>123</v>
       </c>
-      <c r="D19" s="67" t="s">
+      <c r="D19" s="71" t="s">
         <v>126</v>
       </c>
       <c r="E19" s="30" t="s">
@@ -3927,9 +3988,9 @@
       <c r="H19" s="49"/>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B20" s="62"/>
-      <c r="C20" s="65"/>
-      <c r="D20" s="69"/>
+      <c r="B20" s="66"/>
+      <c r="C20" s="69"/>
+      <c r="D20" s="73"/>
       <c r="E20" s="30" t="s">
         <v>103</v>
       </c>
@@ -3942,9 +4003,9 @@
       <c r="H20" s="49"/>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B21" s="62"/>
-      <c r="C21" s="65"/>
-      <c r="D21" s="69"/>
+      <c r="B21" s="66"/>
+      <c r="C21" s="69"/>
+      <c r="D21" s="73"/>
       <c r="E21" s="30" t="s">
         <v>127</v>
       </c>
@@ -3957,13 +4018,13 @@
       <c r="H21" s="49"/>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B22" s="61">
+      <c r="B22" s="65">
         <v>8</v>
       </c>
-      <c r="C22" s="64" t="s">
+      <c r="C22" s="68" t="s">
         <v>105</v>
       </c>
-      <c r="D22" s="67" t="s">
+      <c r="D22" s="71" t="s">
         <v>106</v>
       </c>
       <c r="E22" s="30" t="s">
@@ -3978,9 +4039,9 @@
       <c r="H22" s="49"/>
     </row>
     <row r="23" spans="2:8" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="B23" s="62"/>
-      <c r="C23" s="65"/>
-      <c r="D23" s="68"/>
+      <c r="B23" s="66"/>
+      <c r="C23" s="69"/>
+      <c r="D23" s="72"/>
       <c r="E23" s="30" t="s">
         <v>130</v>
       </c>
@@ -3995,8 +4056,8 @@
       </c>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B24" s="63"/>
-      <c r="C24" s="66"/>
+      <c r="B24" s="67"/>
+      <c r="C24" s="70"/>
       <c r="D24" s="40" t="s">
         <v>108</v>
       </c>
@@ -4014,13 +4075,13 @@
       </c>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B25" s="61">
+      <c r="B25" s="65">
         <v>9</v>
       </c>
-      <c r="C25" s="64" t="s">
+      <c r="C25" s="68" t="s">
         <v>49</v>
       </c>
-      <c r="D25" s="67" t="s">
+      <c r="D25" s="71" t="s">
         <v>110</v>
       </c>
       <c r="E25" s="30" t="s">
@@ -4035,9 +4096,9 @@
       <c r="H25" s="49"/>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B26" s="62"/>
-      <c r="C26" s="65"/>
-      <c r="D26" s="69"/>
+      <c r="B26" s="66"/>
+      <c r="C26" s="69"/>
+      <c r="D26" s="73"/>
       <c r="E26" s="30" t="s">
         <v>109</v>
       </c>
@@ -4050,9 +4111,9 @@
       <c r="H26" s="49"/>
     </row>
     <row r="27" spans="2:8" ht="33" x14ac:dyDescent="0.3">
-      <c r="B27" s="63"/>
-      <c r="C27" s="66"/>
-      <c r="D27" s="68"/>
+      <c r="B27" s="67"/>
+      <c r="C27" s="70"/>
+      <c r="D27" s="72"/>
       <c r="E27" s="30" t="s">
         <v>131</v>
       </c>
@@ -4067,10 +4128,10 @@
       </c>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B28" s="61">
+      <c r="B28" s="65">
         <v>10</v>
       </c>
-      <c r="C28" s="64" t="s">
+      <c r="C28" s="68" t="s">
         <v>111</v>
       </c>
       <c r="D28" s="4" t="s">
@@ -4088,9 +4149,9 @@
       <c r="H28" s="49"/>
     </row>
     <row r="29" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B29" s="62"/>
-      <c r="C29" s="65"/>
-      <c r="D29" s="64" t="s">
+      <c r="B29" s="66"/>
+      <c r="C29" s="69"/>
+      <c r="D29" s="68" t="s">
         <v>113</v>
       </c>
       <c r="E29" s="4" t="s">
@@ -4105,9 +4166,9 @@
       <c r="H29" s="48"/>
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B30" s="63"/>
-      <c r="C30" s="66"/>
-      <c r="D30" s="66"/>
+      <c r="B30" s="67"/>
+      <c r="C30" s="70"/>
+      <c r="D30" s="70"/>
       <c r="E30" s="6" t="s">
         <v>115</v>
       </c>
@@ -4122,13 +4183,13 @@
       </c>
     </row>
     <row r="31" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B31" s="61">
+      <c r="B31" s="65">
         <v>11</v>
       </c>
-      <c r="C31" s="64" t="s">
+      <c r="C31" s="68" t="s">
         <v>51</v>
       </c>
-      <c r="D31" s="67" t="s">
+      <c r="D31" s="71" t="s">
         <v>117</v>
       </c>
       <c r="E31" s="30" t="s">
@@ -4143,9 +4204,9 @@
       <c r="H31" s="49"/>
     </row>
     <row r="32" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B32" s="63"/>
-      <c r="C32" s="66"/>
-      <c r="D32" s="68"/>
+      <c r="B32" s="67"/>
+      <c r="C32" s="70"/>
+      <c r="D32" s="72"/>
       <c r="E32" s="30" t="s">
         <v>118</v>
       </c>
@@ -4222,7 +4283,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <selection activeCell="K24" sqref="K24"/>
+      <selection activeCell="F35" sqref="F35:F36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -4241,4 +4302,107 @@
   </colBreaks>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B4:D17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="4" max="4" width="53.625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B4" s="62" t="s">
+        <v>134</v>
+      </c>
+      <c r="C4" s="62"/>
+      <c r="D4" s="62"/>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B5" s="62"/>
+      <c r="C5" s="62" t="s">
+        <v>135</v>
+      </c>
+      <c r="D5" s="62" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B6" s="62"/>
+      <c r="C6" s="62" t="s">
+        <v>137</v>
+      </c>
+      <c r="D6" s="62" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B7" s="62"/>
+      <c r="C7" s="62"/>
+      <c r="D7" s="62" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B8" s="62"/>
+      <c r="C8" s="62"/>
+      <c r="D8" s="62" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B9" s="62"/>
+      <c r="C9" s="62"/>
+      <c r="D9" s="62" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" ht="82.5" x14ac:dyDescent="0.3">
+      <c r="B10" s="62"/>
+      <c r="C10" s="62"/>
+      <c r="D10" s="63" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B11" s="62"/>
+      <c r="C11" s="62"/>
+      <c r="D11" s="62" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B14" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C15" t="s">
+        <v>145</v>
+      </c>
+      <c r="D15" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4" ht="66" x14ac:dyDescent="0.3">
+      <c r="D16" s="63" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="17" spans="4:4" ht="33" x14ac:dyDescent="0.3">
+      <c r="D17" s="63" t="s">
+        <v>148</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>